<commit_message>
Added intro and cleaned up
Cleanup and spruce up - removed commented lines of code, added comments, changed variable names to better reflect their use, added caching of tracker and colour excel files.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivekctongaonkar/Desktop/Raajas/stre/Mapping ProMED alerts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAB8673-1751-754B-BCDA-F7421CE3329D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D92AF1B-61E0-AA48-B057-4F4E8208E278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{92CE9DDE-4BD2-7A4E-AAC1-76E35D57A2E8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
   <si>
     <t>No.</t>
   </si>
@@ -561,16 +561,30 @@
   </si>
   <si>
     <t>https://promedmail.org/promed-post/?id=8716088</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>https://promedmail.org/promed-post/?id=8716106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -599,16 +613,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -941,11 +958,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1213CEB4-1ED8-6342-9CC0-AA460BE39C43}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1048,7 +1065,7 @@
       <c r="L2" s="1">
         <v>45370</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1241,7 +1258,7 @@
       <c r="L7" s="1">
         <v>45389</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3">
         <v>45200</v>
       </c>
       <c r="P7" t="s">
@@ -1282,7 +1299,7 @@
       <c r="L8" s="1">
         <v>45396</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="3">
         <v>45352</v>
       </c>
       <c r="P8" t="s">
@@ -1551,13 +1568,16 @@
       <c r="H15" t="s">
         <v>19</v>
       </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
       <c r="K15" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="1">
         <v>45399</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2584,8 +2604,43 @@
         <v>174</v>
       </c>
     </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43">
+        <v>-13.769389500000001</v>
+      </c>
+      <c r="G43">
+        <v>-172.12004999999999</v>
+      </c>
+      <c r="H43" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" t="s">
+        <v>152</v>
+      </c>
+      <c r="J43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L43" s="1">
+        <v>45405</v>
+      </c>
+      <c r="P43" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="P15" r:id="rId1" xr:uid="{ADB71EF1-975E-354E-918B-F8638F394A3F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>